<commit_message>
- added second bead kit
</commit_message>
<xml_diff>
--- a/database/beadkits.xlsx
+++ b/database/beadkits.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/welshjoa/Documents/MATLAB/Software Updates/database/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{193AAA31-3D6C-5746-B91B-D55FE5A4C7BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F228E8DD-B16A-724C-8BAE-AA650B90ED95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11840" yWindow="10800" windowWidth="28040" windowHeight="17440" xr2:uid="{104763D7-C1D4-064D-A1D7-9C28DD1D121A}"/>
   </bookViews>
@@ -98,12 +98,6 @@
     <t>L202211</t>
   </si>
   <si>
-    <t>81, 100, 125, 150, 240, 303, 401</t>
-  </si>
-  <si>
-    <t>12, 6.8, 3.3, 3.1, 1.5, 1.6, 1.3</t>
-  </si>
-  <si>
     <t>1.59, 1.59, 1.59, 1.59, 1.59, 1.59, 1.59</t>
   </si>
   <si>
@@ -111,6 +105,12 @@
   </si>
   <si>
     <t>Polystyrene, Polystyrene, Polystyrene, Polystyrene, Polystyrene, Polystyrene, Polystyrene</t>
+  </si>
+  <si>
+    <t>81, 100, 122, 150, 240, 303, 401</t>
+  </si>
+  <si>
+    <t>12, 6.8, 5.6, 3.1, 1.5, 1.6, 1.3</t>
   </si>
 </sst>
 </file>
@@ -465,7 +465,7 @@
   <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -545,22 +545,22 @@
         <v>12</v>
       </c>
       <c r="D3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" t="s">
         <v>20</v>
       </c>
-      <c r="E3" t="s">
+      <c r="G3" t="s">
         <v>21</v>
-      </c>
-      <c r="F3" t="s">
-        <v>22</v>
-      </c>
-      <c r="G3" t="s">
-        <v>23</v>
       </c>
       <c r="H3" t="s">
         <v>17</v>
       </c>
       <c r="I3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="J3">
         <v>220</v>

</xml_diff>